<commit_message>
Add census/calf proportion as data instead of bpt_analyse() function arguments
</commit_message>
<xml_diff>
--- a/inst/example-data/data-raw.xlsx
+++ b/inst/example-data/data-raw.xlsx
@@ -1,27 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolehill/Code/bisonpictools/data-raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolehill/Code/bisonpictools/inst/example-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E3C1DF-1257-8A4D-AB37-DB41247FA063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF475C5B-AA2B-8D44-8708-1166B1034B98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="25320" windowHeight="13920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="25320" windowHeight="13920" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="location" sheetId="1" r:id="rId1"/>
     <sheet name="event" sheetId="2" r:id="rId2"/>
+    <sheet name="census" sheetId="3" r:id="rId3"/>
+    <sheet name="proportion_calf" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="36">
   <si>
     <t>location_id</t>
   </si>
@@ -99,13 +101,43 @@
   </si>
   <si>
     <t>LOCID4</t>
+  </si>
+  <si>
+    <t>proportion_calf_year</t>
+  </si>
+  <si>
+    <t>proportion_calf_month</t>
+  </si>
+  <si>
+    <t>proportion_calf_day</t>
+  </si>
+  <si>
+    <t>proportion_calf</t>
+  </si>
+  <si>
+    <t>proportion_calf_cv</t>
+  </si>
+  <si>
+    <t>census_year</t>
+  </si>
+  <si>
+    <t>census_month</t>
+  </si>
+  <si>
+    <t>census_day</t>
+  </si>
+  <si>
+    <t>census</t>
+  </si>
+  <si>
+    <t>census_cv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,6 +155,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -148,11 +187,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -533,7 +573,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="200" workbookViewId="0">
+    <sheetView zoomScale="91" zoomScaleNormal="200" workbookViewId="0">
       <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
@@ -1353,4 +1393,143 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8DF943C-64A7-A14D-A0AA-820EF9B7FFE8}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2021</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2">
+        <v>31</v>
+      </c>
+      <c r="D2" s="2">
+        <v>250</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2022</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>31</v>
+      </c>
+      <c r="D3">
+        <v>275</v>
+      </c>
+      <c r="E3">
+        <v>0.06</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AE92973-1862-9A44-A299-EF2CD865374F}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2021</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2">
+        <v>31</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2022</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>31</v>
+      </c>
+      <c r="D3">
+        <v>0.15</v>
+      </c>
+      <c r="E3">
+        <v>0.09</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>